<commit_message>
Added code to read in data from exel file and use it to construct planets
</commit_message>
<xml_diff>
--- a/java/data/Planets.xlsx
+++ b/java/data/Planets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BF0884-EBC0-4F6F-95CF-2BDD2DE96DB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00200F36-633D-435C-AC52-542BFCA5A2E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -80,13 +80,43 @@
   </si>
   <si>
     <t>Hadrian</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Planet1</t>
+  </si>
+  <si>
+    <t>Planet2</t>
+  </si>
+  <si>
+    <t>Planet3</t>
+  </si>
+  <si>
+    <t>Planet4</t>
+  </si>
+  <si>
+    <t>Planet5</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, , </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +135,24 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF4EC9B0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -137,6 +185,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,187 +474,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>650</v>
+      </c>
+      <c r="E2">
+        <v>90</v>
+      </c>
+      <c r="F2" s="4">
         <v>2.1040000000000001</v>
       </c>
-      <c r="C2" s="4">
+      <c r="G2" s="4">
         <v>2.036</v>
       </c>
-      <c r="D2" s="4">
+      <c r="H2" s="4">
         <v>0.56899999999999995</v>
       </c>
-      <c r="E2" s="4">
+      <c r="I2" s="4">
         <v>0.10299999999999999</v>
       </c>
-      <c r="F2" s="4">
+      <c r="J2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="4">
+      <c r="K2" s="4">
         <v>346.03800000000001</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4">
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3">
+        <v>350</v>
+      </c>
+      <c r="E3">
+        <v>190</v>
+      </c>
+      <c r="F3" s="4">
         <v>0.97299999999999998</v>
       </c>
-      <c r="C3" s="4">
+      <c r="G3" s="4">
         <v>23.056000000000001</v>
       </c>
-      <c r="D3" s="4">
+      <c r="H3" s="4">
         <v>24.689</v>
       </c>
-      <c r="E3" s="4">
+      <c r="I3" s="4">
         <v>10.456</v>
       </c>
-      <c r="F3" s="4">
+      <c r="J3" s="4">
         <v>2.3519999999999999</v>
       </c>
-      <c r="G3" s="4">
+      <c r="K3" s="4">
         <v>456.35599999999999</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4">
+      <c r="C4">
+        <v>150</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4" s="4">
         <v>5.8970000000000002</v>
       </c>
-      <c r="C4" s="4">
+      <c r="G4" s="4">
         <v>10.459</v>
       </c>
-      <c r="D4" s="4">
+      <c r="H4" s="4">
         <v>14.651</v>
       </c>
-      <c r="E4" s="4">
+      <c r="I4" s="4">
         <v>0.105</v>
       </c>
-      <c r="F4" s="4">
+      <c r="J4" s="4">
         <v>30.571999999999999</v>
       </c>
-      <c r="G4" s="4">
+      <c r="K4" s="4">
         <v>205.76400000000001</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4">
+      <c r="C5">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5">
+        <v>300</v>
+      </c>
+      <c r="F5" s="4">
         <v>0.64800000000000002</v>
       </c>
-      <c r="C5" s="4">
+      <c r="G5" s="4">
         <v>40.341000000000001</v>
       </c>
-      <c r="D5" s="4">
+      <c r="H5" s="4">
         <v>10.054</v>
       </c>
-      <c r="E5" s="4">
+      <c r="I5" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="J5" s="4">
         <v>10.763999999999999</v>
       </c>
-      <c r="G5" s="4">
+      <c r="K5" s="4">
         <v>298.45600000000002</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4">
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>810</v>
+      </c>
+      <c r="E6">
+        <v>300</v>
+      </c>
+      <c r="F6" s="4">
         <v>8.5660000000000007</v>
       </c>
-      <c r="C6" s="4">
+      <c r="G6" s="4">
         <v>20.451000000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="H6" s="4">
         <v>13.569000000000001</v>
       </c>
-      <c r="E6" s="4">
+      <c r="I6" s="4">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="J6" s="4">
         <v>15.782999999999999</v>
       </c>
-      <c r="G6" s="4">
+      <c r="K6" s="4">
         <v>134.768</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C12" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>